<commit_message>
New card action text display
Made it so that the program will underline the "emphasis" of a cards actions instead of needing to bold and underline the text in the spreadsheet.

Updated spreadsheet to reflect changes to program. Split command card actions to:
Action Emphasis and Action Text
</commit_message>
<xml_diff>
--- a/Main/NEW_PROTOCOL/Compile.xlsx
+++ b/Main/NEW_PROTOCOL/Compile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Protocol Name</t>
   </si>
@@ -47,13 +47,22 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Persistent</t>
-  </si>
-  <si>
-    <t>Immediate</t>
-  </si>
-  <si>
-    <t>Auxiliary</t>
+    <t>Persistent Emphasis</t>
+  </si>
+  <si>
+    <t>Persistent Text</t>
+  </si>
+  <si>
+    <t>Immediate Emphasis</t>
+  </si>
+  <si>
+    <t>Immediate Text</t>
+  </si>
+  <si>
+    <t>Auxiliary Emphasis</t>
+  </si>
+  <si>
+    <t>Auxiliary Text</t>
   </si>
   <si>
     <t>v0.1</t>
@@ -62,22 +71,10 @@
     <t>Card 1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <u/>
-      </rPr>
-      <t>If your cards shift:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> Draw 1 card.</t>
-    </r>
+    <t>If your cards shift</t>
+  </si>
+  <si>
+    <t>Draw 1 card.</t>
   </si>
   <si>
     <t>Draw 3 cards.</t>
@@ -86,43 +83,13 @@
     <t>Card 2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <u/>
-      </rPr>
-      <t>Start:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> Draw 1 card.</t>
-    </r>
+    <t>Start</t>
   </si>
   <si>
     <t>Card 3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <u/>
-      </rPr>
-      <t>When this card is covered:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> Draw 1 card.</t>
-    </r>
+    <t>When this card is covered</t>
   </si>
   <si>
     <t>Shift any 2 cards to this line.</t>
@@ -131,22 +98,10 @@
     <t>Card 4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <u/>
-      </rPr>
-      <t>When your opponent draws cards:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> Shift 1 of their cards.</t>
-    </r>
+    <t>When your opponent draws cards</t>
+  </si>
+  <si>
+    <t>Shift 1 of their cards.</t>
   </si>
   <si>
     <t>Card 5</t>
@@ -165,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -176,17 +131,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,13 +140,31 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -212,17 +174,23 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,128 +463,167 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="14.38"/>
     <col customWidth="1" min="3" max="3" width="6.38"/>
-    <col customWidth="1" min="4" max="6" width="47.63"/>
+    <col customWidth="1" min="4" max="4" width="27.5"/>
+    <col customWidth="1" min="5" max="5" width="47.63"/>
+    <col customWidth="1" min="6" max="6" width="18.38"/>
+    <col customWidth="1" min="7" max="7" width="22.25"/>
+    <col customWidth="1" min="8" max="9" width="47.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7">
         <v>0.0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7">
         <v>1.0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7">
         <v>3.0</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7">
         <v>4.0</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7">
         <v>5.0</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>